<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@f26a8cc4ea975c29de952cf2507fdae0caea5eb9 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-uscore-treatment-intervention-preference.xlsx
+++ b/CodeSystem-uscore-treatment-intervention-preference.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/uscdi4-sandbox/CodeSystem/uscore-treatment-intervention-preference</t>
+    <t>http://hl7.org/fhir/us/core/CodeSystem/uscore-treatment-intervention-preference</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-31T01:42:33.501000+00:00</t>
+    <t>2023-10-02</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>